<commit_message>
deleted close browser line code in DuplicateLead And modified data in excel
</commit_message>
<xml_diff>
--- a/SeleniumLearning/data/MergeLead.xlsx
+++ b/SeleniumLearning/data/MergeLead.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Promantus\Downloads\eclipse_64bit\eclipse_64bit\SeleniumLearning\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Promantus\git\SeleniumJune2021\SeleniumLearning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7159BD40-5ABC-4367-9AB2-4C1B53C31CDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3460D4E-5886-4D09-AB21-D0856F1CFECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{16376A58-C88A-4E27-BA61-4BEF299276C5}"/>
   </bookViews>
@@ -33,33 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>firstName</t>
   </si>
   <si>
-    <t>Amali</t>
+    <t>Lekha</t>
   </si>
   <si>
-    <t>John</t>
+    <t>Priya</t>
   </si>
   <si>
-    <t>Suresh</t>
-  </si>
-  <si>
-    <t>Alvin</t>
-  </si>
-  <si>
-    <t>Joel</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>Matthew</t>
+    <t>Hari</t>
   </si>
 </sst>
 </file>
@@ -421,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E16B010-D2A5-4980-BEA4-79D7CA62DAB5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,44 +417,24 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>